<commit_message>
Reduce reserved keys for fields to bare minimum
</commit_message>
<xml_diff>
--- a/media/test_imports/reserved_field_key.xlsx
+++ b/media/test_imports/reserved_field_key.xlsx
@@ -16,7 +16,7 @@
     <t>URN:Tel</t>
   </si>
   <si>
-    <t>Field:id</t>
+    <t>Field:HAS</t>
   </si>
   <si>
     <t>12</t>
@@ -53,9 +53,9 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="15"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -72,7 +72,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -95,13 +95,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -114,8 +151,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -362,7 +408,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -392,7 +437,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -418,7 +462,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -444,7 +487,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -470,7 +512,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -496,7 +537,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -522,7 +562,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -548,7 +587,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -574,7 +612,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -600,7 +637,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -651,7 +687,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -677,7 +712,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -703,7 +737,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -729,7 +762,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -755,7 +787,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -781,7 +812,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -807,7 +837,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -833,7 +862,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -859,7 +887,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -885,7 +912,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -933,7 +959,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -963,7 +988,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -989,7 +1013,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1015,7 +1038,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1041,7 +1063,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1067,7 +1088,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1093,7 +1113,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1119,7 +1138,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1145,7 +1163,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1171,7 +1188,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1197,7 +1213,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1205,7 +1221,8 @@
   <cols>
     <col min="1" max="1" width="12.8516" style="1" customWidth="1"/>
     <col min="2" max="4" width="10.3516" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.8516" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1217,9 +1234,10 @@
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="20" customHeight="1">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <v>250788382382</v>
       </c>
       <c r="B2" t="s" s="2">
@@ -1227,6 +1245,7 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="2">
@@ -1237,6 +1256,7 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="2">
@@ -1247,42 +1267,49 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" ht="14.65" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" ht="14.65" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" ht="14.65" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" ht="14.65" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" ht="14.65" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" ht="14.65" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.25" footer="0.25"/>

</xml_diff>